<commit_message>
Selenium Season 3 Nov 1st
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/regression/Adactin Master Test Data.xlsx
+++ b/src/test/resources/testdata/excels/regression/Adactin Master Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FLM31stJulWS\HybridFrameWork\src\test\resources\testdata\excels\regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1469E6AC-71D5-4BD4-8848-4F4D87758792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0A4DDD-0639-43B5-BA03-6D32FDEA1736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ECA7341F-7CE3-4EA7-B2BF-C9C26B540FCF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
   <si>
     <t>username</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>reyaz009</t>
+  </si>
+  <si>
+    <t>Ravi0111</t>
+  </si>
+  <si>
+    <t>Adactin.com - New User Registration</t>
   </si>
 </sst>
 </file>
@@ -551,14 +557,14 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -604,21 +610,24 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -627,21 +636,24 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -730,7 +742,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{339D628B-76D7-4244-B40A-3F8AEE44D028}"/>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{339D628B-76D7-4244-B40A-3F8AEE44D028}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>